<commit_message>
DHS update Chapter 9 - RH
DHS8 update to Reproductive Health (Maternal Health) indicators
</commit_message>
<xml_diff>
--- a/IndicatorList_DHS8.xlsx
+++ b/IndicatorList_DHS8.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/Shared Resources/Code/DHS-Indicators-Stata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="850" documentId="114_{17F82F54-F8CB-43F8-AF09-BA1DBACED508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{493441F9-A1DA-41E2-89F2-5407AEB4C4EF}"/>
+  <xr:revisionPtr revIDLastSave="856" documentId="114_{17F82F54-F8CB-43F8-AF09-BA1DBACED508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02C85E7B-21C3-4A20-AF0C-99C5C14755CB}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" tabRatio="690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" tabRatio="690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ch7FP" sheetId="5" r:id="rId1"/>
+    <sheet name="Ch9RH" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="446">
   <si>
     <t>Chapter</t>
   </si>
@@ -940,6 +941,442 @@
   </si>
   <si>
     <t>"Women non-users who did not discuss FP neither with FP worker or in a health facility in last 12 months"</t>
+  </si>
+  <si>
+    <t>Reproductive Health</t>
+  </si>
+  <si>
+    <t>RHmain.do</t>
+  </si>
+  <si>
+    <t>Main file for the reproductive health chapter. The main file will call the do files listed below and the RH_tables.do file not listed here. The tables do file will produce excel tables of the indicators.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In DHS8, use NR file and p19 and m80 to select women. The indicators below are computed for women with a live and/or stillbirth in the 2 years before the survey. Please read notes in the do files and main do file.  </t>
+  </si>
+  <si>
+    <t>RH_ANC.do</t>
+  </si>
+  <si>
+    <t>rh_anc_pv</t>
+  </si>
+  <si>
+    <t>"Person providing assistance during ANC"</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is country specific and needs to be checked. </t>
+  </si>
+  <si>
+    <t>rh_anc_pvskill</t>
+  </si>
+  <si>
+    <t>"Skilled assistance during ANC"</t>
+  </si>
+  <si>
+    <t>This is country specific and needs to be checked. Variable was changed to a binary variable.</t>
+  </si>
+  <si>
+    <t>rh_anc_numvs</t>
+  </si>
+  <si>
+    <t>"Number of ANC visits"</t>
+  </si>
+  <si>
+    <t>rh_anc_4vs</t>
+  </si>
+  <si>
+    <t>"Attended 4+ ANC visits"</t>
+  </si>
+  <si>
+    <t>rh_anc_moprg</t>
+  </si>
+  <si>
+    <t>"Number of months pregnant at  time of first ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_median</t>
+  </si>
+  <si>
+    <t>Median months pregnant at first visit - among live births + stillbirths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a scalar not a variable </t>
+  </si>
+  <si>
+    <t>rh_anc_median_liveb</t>
+  </si>
+  <si>
+    <t>Median months pregnant at first visit - among live births</t>
+  </si>
+  <si>
+    <t>This is a scalar not a variable - NEW Indicator in DHS8</t>
+  </si>
+  <si>
+    <t>rh_anc_median_stillb</t>
+  </si>
+  <si>
+    <t>Median months pregnant at first visit - among stillbirths</t>
+  </si>
+  <si>
+    <t>rh_anc_bldpres</t>
+  </si>
+  <si>
+    <t>"Blood pressure was taken during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_urine</t>
+  </si>
+  <si>
+    <t>"Urine sample was taken during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_bldsamp</t>
+  </si>
+  <si>
+    <t>"Blood sample was taken during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_heartbt</t>
+  </si>
+  <si>
+    <t>"Baby's heartbeat was listened for during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_consldiet</t>
+  </si>
+  <si>
+    <t>"Counseled about maternal diet during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_conslbf</t>
+  </si>
+  <si>
+    <t>"Counseled about breastfeeding during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_askvagbleed</t>
+  </si>
+  <si>
+    <t>"Asked about vaginal bleeding during ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_anc_iron</t>
+  </si>
+  <si>
+    <t>"Took iron tablet/syrup during most recent pregnancy"</t>
+  </si>
+  <si>
+    <t>rh_anc_parast</t>
+  </si>
+  <si>
+    <t>"Took intestinal parasite drugs during most recent pregnancy"</t>
+  </si>
+  <si>
+    <t>rh_anc_foodcash</t>
+  </si>
+  <si>
+    <t>"Took food or cash assistance during most recent pregnancy"</t>
+  </si>
+  <si>
+    <t>rh_anc_daysiron</t>
+  </si>
+  <si>
+    <t>"Number of days took iron-containing supplements during most recent pregnancy"</t>
+  </si>
+  <si>
+    <t>rh_anc_ironpl_(a-x)</t>
+  </si>
+  <si>
+    <t>"Place where iron-continaining supplements where obtained: xx"</t>
+  </si>
+  <si>
+    <t>NEW Indicator in DHS8
+This is a country specific variable which depends on the number of sources available. The code will produce a vairable for each source in the survey from a to x</t>
+  </si>
+  <si>
+    <t>rh_anc_toxinj</t>
+  </si>
+  <si>
+    <t>"Received 2+ tetanus injections during last pregnancy"</t>
+  </si>
+  <si>
+    <t>rh_anc_neotet</t>
+  </si>
+  <si>
+    <t>"Protected against neonatal tetanus"</t>
+  </si>
+  <si>
+    <t>RH_PNC.do</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_timing</t>
+  </si>
+  <si>
+    <t>"Timing after delivery for mother's PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_2days</t>
+  </si>
+  <si>
+    <t>"PNC check within two days for mother"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_pv</t>
+  </si>
+  <si>
+    <t>"Provider for mother's PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_bldpres</t>
+  </si>
+  <si>
+    <t>"Blood pressure was taken during PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_askvagbleed</t>
+  </si>
+  <si>
+    <t>"Discussed vaginal bleeding during PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_fp</t>
+  </si>
+  <si>
+    <t>"Discussed family planning during PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_wm_allchecks</t>
+  </si>
+  <si>
+    <t>"All three checks were made duirng PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_timing</t>
+  </si>
+  <si>
+    <t>"Timing after delivery for newborn's PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_2days</t>
+  </si>
+  <si>
+    <t>"PNC check within two days for newborn"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_pv</t>
+  </si>
+  <si>
+    <t>"Provider for newborn's PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_cord</t>
+  </si>
+  <si>
+    <t>"Examined cord during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_temp</t>
+  </si>
+  <si>
+    <t>"Measured temperature during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_dngr</t>
+  </si>
+  <si>
+    <t>"Mother told how to recognize if baby needs immediate medical attention during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_conslbf</t>
+  </si>
+  <si>
+    <t>"Mother counseled on breastfeeding during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_obsbf</t>
+  </si>
+  <si>
+    <t>"Observed breastfeeding during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_conslobsbf</t>
+  </si>
+  <si>
+    <t>"Counseled and observed breastfeeding during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_weighed</t>
+  </si>
+  <si>
+    <t>"Weighed during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_nb_5sigfunc</t>
+  </si>
+  <si>
+    <t>"Performed five or more signal postnatal care fucntions during newborn PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_bothchecked</t>
+  </si>
+  <si>
+    <t>"Both mother and newborn received a PNC check"</t>
+  </si>
+  <si>
+    <t>rh_pnc_bothnotchecked</t>
+  </si>
+  <si>
+    <t>"Neither mother nor newborn received a PNC check"</t>
+  </si>
+  <si>
+    <t>RH_DEL.do</t>
+  </si>
+  <si>
+    <t>rh_del_facil</t>
+  </si>
+  <si>
+    <t>"Live births delivered in a health facility"</t>
+  </si>
+  <si>
+    <t>This was changed to a binary variable for health facility delivery</t>
+  </si>
+  <si>
+    <t>rh_del_pltype</t>
+  </si>
+  <si>
+    <t>"Live births by type of health facility"</t>
+  </si>
+  <si>
+    <t>This was changed to include separate categories for private NGO and non-NGO. Please check country specific categories</t>
+  </si>
+  <si>
+    <t>rh_del_pv</t>
+  </si>
+  <si>
+    <t>"Person providing assistance during birth"</t>
+  </si>
+  <si>
+    <t>rh_del_pvskill</t>
+  </si>
+  <si>
+    <t>"Skilled provider providing assistance during birth"</t>
+  </si>
+  <si>
+    <t>rh_del_skin</t>
+  </si>
+  <si>
+    <t>"Births with skin-to-skin contact immediately after birth"</t>
+  </si>
+  <si>
+    <t>This was missing in DHS7 code, it's not a new indicator but was missing in the code.</t>
+  </si>
+  <si>
+    <t>rh_del_ces</t>
+  </si>
+  <si>
+    <t>"Births delivered by cesarean"</t>
+  </si>
+  <si>
+    <t>rh_del_cestime</t>
+  </si>
+  <si>
+    <t>"Timing of decision to have Cesarean"</t>
+  </si>
+  <si>
+    <t>rh_del_stay</t>
+  </si>
+  <si>
+    <t>"Duration of stay following recent birth"</t>
+  </si>
+  <si>
+    <t>RH_HLTH.do</t>
+  </si>
+  <si>
+    <t>rh_brst_cncr_exam</t>
+  </si>
+  <si>
+    <t>"Ever examined by health worker for breast cancer"</t>
+  </si>
+  <si>
+    <t>rh_cervc_cancr_test</t>
+  </si>
+  <si>
+    <t>"Ever tested for cervical cancer"</t>
+  </si>
+  <si>
+    <t>rh_prob_permit</t>
+  </si>
+  <si>
+    <t>"Problem health care access: permission to go"</t>
+  </si>
+  <si>
+    <t>rh_prob_money</t>
+  </si>
+  <si>
+    <t>"Problem health care access: getting money"</t>
+  </si>
+  <si>
+    <t>rh_prob_dist</t>
+  </si>
+  <si>
+    <t>"Problem health care access: distance to facility"</t>
+  </si>
+  <si>
+    <t>rh_prob_alone</t>
+  </si>
+  <si>
+    <t>"Problem health care access: not wanting to go alone"</t>
+  </si>
+  <si>
+    <t>rh_prob_minone</t>
+  </si>
+  <si>
+    <t>"At least one problem in accessing health care"</t>
+  </si>
+  <si>
+    <t>rh_traveltime_hlthfacil</t>
+  </si>
+  <si>
+    <t>"Travel time to nearest health facility"</t>
+  </si>
+  <si>
+    <t>rh_transport_hlthfacil</t>
+  </si>
+  <si>
+    <t>"Means of transport to nearest facility"</t>
+  </si>
+  <si>
+    <t>RH_MEN.do</t>
+  </si>
+  <si>
+    <t>rh_mn_report_anc</t>
+  </si>
+  <si>
+    <t>"Report that their child's mother had any ANC"</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>rh_mn_present_anc</t>
+  </si>
+  <si>
+    <t>"Present during any ANC visit"</t>
+  </si>
+  <si>
+    <t>rh_mn_report_delfacil</t>
+  </si>
+  <si>
+    <t>"Report that their child was born in health facility"</t>
+  </si>
+  <si>
+    <t>rh_mn_present_delfacil</t>
+  </si>
+  <si>
+    <t>"Went with child's mother to health facility for delivery"</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1012,6 +1449,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1029,10 +1479,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1300,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3483,6 +3929,1108 @@
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="F31:F48"/>
     <mergeCell ref="F94:F107"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89EE9364-F6EF-4839-BD00-B07BD7221DCA}">
+  <dimension ref="A1:F75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="67.54296875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="65.1796875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="38.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F56" s="9"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F57" s="9"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="E60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" s="9"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="9"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" s="9"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B72" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B73" s="9"/>
+      <c r="C73" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B74" s="9"/>
+      <c r="C74" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3790,34 +5338,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-33084</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-33084</Url>
-      <Description>VMX3MACP777Z-432858100-33084</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3867,6 +5387,34 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-33084</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-33084</Url>
+      <Description>VMX3MACP777Z-432858100-33084</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7400C4A1-7880-4671-9CBA-143AD7B24860}">
   <ds:schemaRefs>
@@ -3889,14 +5437,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
-    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
-    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3910,9 +5453,14 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
+    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
+    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>